<commit_message>
Aggiornamento test [24, 25, 26, 27, 6, 7, 8, 9]
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#070103000000XX/ASL3_Genovese/SIVIS/v.1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#070103000000XX/ASL3_Genovese/SIVIS/v.1.0.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabat\Desktop\FSE Test case\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabat\PhpstormProjects\it-fse-accreditamento\GATEWAY\A1#070103000000XX\ASL3_Genovese\SIVIS\v.1.0.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA3CC53-1550-47AA-AAD7-441909ACF75B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AB215A-EB38-4C13-9248-1156B8E44C8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -758,12 +758,6 @@
     </r>
   </si>
   <si>
-    <t>12672e2846867c5f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.a57bffedf8856b64c95e946e1ec3c8081182223cad34d0dadec5d50f8da09c18.5b5aadfa26^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>b1c585158ec44531</t>
   </si>
   <si>
@@ -857,30 +851,6 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.a57bffedf8856b64c95e946e1ec3c8081182223cad34d0dadec5d50f8da09c18.99f389e4db^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>b9febbe1cddebe23</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.68e476b5d5aeca7b0e3b5ca867106c32e40cad05a490f6b08a24063cceed7e7e.b4b13f45dc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>561e429bd758b177</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.fcf1e4bf9cc9c1083647b91463e86f49c6961406c37055c7eb8ad13937a519db.a5ec9182c9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>0bc2a46fa4760528</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.bf7db3a1fea244ba0c173404b5abb382def24d3bc547ca4f410bae2a311cdf85.7ac27dfb42^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f898b9bb4e5c2d1d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.182dc6b90f1c9cd913c39a6b5506f582caba9ddeadafe32f5bdbac25efd705ac.2821430401^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>970eb2ed49393494</t>
   </si>
   <si>
@@ -1158,6 +1128,36 @@
   </si>
   <si>
     <t>Viene segnalato all'operatore l'errore: Errore semantico. [ERRORE-b94|Sezione Terapia farmacologica alla dimissione: section\/entry\/substanceAdministration\/effectiveTime deve avere l'elemento 'low' valorizzato ],[ERRORE-b95|Sezione Terapia farmacologica alla dimissione: section\/entry\/substanceAdministration\/effectiveTime\/high deve essere presente solo nel caso in cui lo 'statusCode' sia 'completed'oppure'aborted']</t>
+  </si>
+  <si>
+    <t>581801d64fb2a942</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.68e476b5d5aeca7b0e3b5ca867106c32e40cad05a490f6b08a24063cceed7e7e.321b9779d5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>244ff80ca8af6672</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.863a2a5da8e75ced73102148e576def3dea905b8d30d77dbde83119f3a1c4e30.860fdf0424^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3aa91dd4c62f6f44</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.863a2a5da8e75ced73102148e576def3dea905b8d30d77dbde83119f3a1c4e30.1a3a0e3026^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>6b93d7a12a6440c0</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.863a2a5da8e75ced73102148e576def3dea905b8d30d77dbde83119f3a1c4e30.6137c831e7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>cefd0e3c1c7412a1</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.120.4.4.863a2a5da8e75ced73102148e576def3dea905b8d30d77dbde83119f3a1c4e30.b3e4f0a70e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1630,7 +1630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1829,6 +1829,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3199,10 +3202,10 @@
   <dimension ref="A1:O905"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G74" sqref="G74"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3415,16 +3418,16 @@
         <v>31</v>
       </c>
       <c r="F10" s="20">
-        <v>44964</v>
+        <v>44988</v>
       </c>
       <c r="G10" s="43">
-        <v>0.41087962962962959</v>
+        <v>0.41500000000000004</v>
       </c>
       <c r="H10" s="46" t="s">
-        <v>155</v>
+        <v>281</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>156</v>
+        <v>282</v>
       </c>
       <c r="J10" s="22" t="s">
         <v>152</v>
@@ -3439,7 +3442,7 @@
       <c r="N10" s="23"/>
       <c r="O10" s="24"/>
     </row>
-    <row r="11" spans="1:15" ht="14.25" customHeight="1">
+    <row r="11" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
       <c r="A11" s="17">
         <v>7</v>
       </c>
@@ -3462,10 +3465,10 @@
         <v>0.41449074074074077</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J11" s="22" t="s">
         <v>152</v>
@@ -3503,10 +3506,10 @@
         <v>0.42420138888888892</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J12" s="22" t="s">
         <v>152</v>
@@ -3521,7 +3524,7 @@
       <c r="N12" s="23"/>
       <c r="O12" s="24"/>
     </row>
-    <row r="13" spans="1:15" ht="14.25" customHeight="1">
+    <row r="13" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
       <c r="A13" s="17">
         <v>9</v>
       </c>
@@ -3544,10 +3547,10 @@
         <v>0.42925925925925923</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J13" s="22" t="s">
         <v>152</v>
@@ -3562,7 +3565,7 @@
       <c r="N13" s="23"/>
       <c r="O13" s="24"/>
     </row>
-    <row r="14" spans="1:15" ht="147" customHeight="1">
+    <row r="14" spans="1:15" ht="147" customHeight="1" thickBot="1">
       <c r="A14" s="17">
         <v>24</v>
       </c>
@@ -3579,16 +3582,16 @@
         <v>43</v>
       </c>
       <c r="F14" s="20">
-        <v>44964</v>
+        <v>44988</v>
       </c>
       <c r="G14" s="43">
-        <v>0.48298611111111112</v>
+        <v>0.39851851851851849</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>188</v>
+        <v>279</v>
       </c>
       <c r="I14" s="21" t="s">
-        <v>189</v>
+        <v>280</v>
       </c>
       <c r="J14" s="22" t="s">
         <v>152</v>
@@ -3603,7 +3606,7 @@
       <c r="N14" s="23"/>
       <c r="O14" s="24"/>
     </row>
-    <row r="15" spans="1:15" ht="14.25" customHeight="1">
+    <row r="15" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
       <c r="A15" s="17">
         <v>25</v>
       </c>
@@ -3620,16 +3623,16 @@
         <v>45</v>
       </c>
       <c r="F15" s="20">
-        <v>44964</v>
+        <v>44988</v>
       </c>
       <c r="G15" s="44">
-        <v>0.48519675925925926</v>
+        <v>0.41728009259259258</v>
       </c>
       <c r="H15" s="46" t="s">
-        <v>190</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>191</v>
+        <v>283</v>
+      </c>
+      <c r="I15" s="49" t="s">
+        <v>284</v>
       </c>
       <c r="J15" s="22" t="s">
         <v>152</v>
@@ -3644,7 +3647,7 @@
       <c r="N15" s="23"/>
       <c r="O15" s="24"/>
     </row>
-    <row r="16" spans="1:15" ht="14.25" customHeight="1">
+    <row r="16" spans="1:15" ht="14.25" customHeight="1" thickBot="1">
       <c r="A16" s="17">
         <v>26</v>
       </c>
@@ -3661,16 +3664,16 @@
         <v>47</v>
       </c>
       <c r="F16" s="20">
-        <v>44964</v>
+        <v>44988</v>
       </c>
       <c r="G16" s="43">
-        <v>0.48697916666666669</v>
+        <v>0.42005787037037035</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>192</v>
+        <v>285</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>193</v>
+        <v>286</v>
       </c>
       <c r="J16" s="22" t="s">
         <v>152</v>
@@ -3702,16 +3705,16 @@
         <v>49</v>
       </c>
       <c r="F17" s="20">
-        <v>44964</v>
+        <v>44988</v>
       </c>
       <c r="G17" s="52">
-        <v>0.48890046296296297</v>
-      </c>
-      <c r="H17" s="53" t="s">
-        <v>194</v>
+        <v>0.42237268518518517</v>
+      </c>
+      <c r="H17" s="79" t="s">
+        <v>287</v>
       </c>
       <c r="I17" s="53" t="s">
-        <v>195</v>
+        <v>288</v>
       </c>
       <c r="J17" s="54" t="s">
         <v>152</v>
@@ -3749,13 +3752,13 @@
         <v>0.63709490740740737</v>
       </c>
       <c r="H18" s="63" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="I18" s="64" t="s">
         <v>152</v>
       </c>
       <c r="J18" s="63" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="K18" s="22" t="s">
         <v>50</v>
@@ -3792,13 +3795,13 @@
         <v>0.63814814814814813</v>
       </c>
       <c r="H19" s="63" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="I19" s="65" t="s">
         <v>152</v>
       </c>
       <c r="J19" s="63" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="K19" s="22" t="s">
         <v>50</v>
@@ -3835,13 +3838,13 @@
         <v>0.63067129629629626</v>
       </c>
       <c r="H20" s="58" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="I20" s="58" t="s">
         <v>153</v>
       </c>
       <c r="J20" s="59" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="K20" s="22" t="s">
         <v>50</v>
@@ -3878,13 +3881,13 @@
         <v>0.62907407407407401</v>
       </c>
       <c r="H21" s="60" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="I21" s="58" t="s">
         <v>153</v>
       </c>
       <c r="J21" s="59" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="K21" s="22" t="s">
         <v>50</v>
@@ -3927,7 +3930,7 @@
         <v>152</v>
       </c>
       <c r="J22" s="57" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="K22" s="22" t="s">
         <v>50</v>
@@ -3970,7 +3973,7 @@
         <v>152</v>
       </c>
       <c r="J23" s="57" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="K23" s="22" t="s">
         <v>50</v>
@@ -4007,13 +4010,13 @@
         <v>0.43149305555555556</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J24" s="22" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="K24" s="22" t="s">
         <v>50</v>
@@ -4050,13 +4053,13 @@
         <v>0.43532407407407409</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I25" s="21" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="K25" s="22" t="s">
         <v>50</v>
@@ -4093,13 +4096,13 @@
         <v>0.44012731481481482</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J26" s="22" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="K26" s="22" t="s">
         <v>50</v>
@@ -4136,13 +4139,13 @@
         <v>0.44226851851851851</v>
       </c>
       <c r="H27" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I27" s="21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J27" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="K27" s="22" t="s">
         <v>50</v>
@@ -4179,13 +4182,13 @@
         <v>0.4443981481481481</v>
       </c>
       <c r="H28" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I28" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J28" s="22" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="K28" s="22" t="s">
         <v>50</v>
@@ -4222,13 +4225,13 @@
         <v>0.4463078703703704</v>
       </c>
       <c r="H29" s="21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J29" s="22" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="K29" s="22" t="s">
         <v>50</v>
@@ -4265,13 +4268,13 @@
         <v>0.45083333333333336</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="K30" s="22" t="s">
         <v>50</v>
@@ -4308,13 +4311,13 @@
         <v>0.4528240740740741</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J31" s="22" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="K31" s="22" t="s">
         <v>50</v>
@@ -4351,13 +4354,13 @@
         <v>0.45454861111111106</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J32" s="22" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="K32" s="22" t="s">
         <v>50</v>
@@ -4394,13 +4397,13 @@
         <v>0.45699074074074075</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J33" s="22" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="K33" s="22" t="s">
         <v>50</v>
@@ -4434,16 +4437,16 @@
         <v>44964</v>
       </c>
       <c r="G34" s="43" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H34" s="43" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J34" s="22" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="K34" s="22" t="s">
         <v>50</v>
@@ -4480,13 +4483,13 @@
         <v>0.46509259259259261</v>
       </c>
       <c r="H35" s="21" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I35" s="21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J35" s="22" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="K35" s="22" t="s">
         <v>50</v>
@@ -4523,13 +4526,13 @@
         <v>0.49236111111111108</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="J36" s="22" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="K36" s="22" t="s">
         <v>50</v>
@@ -4569,10 +4572,10 @@
         <v>4787274895692470</v>
       </c>
       <c r="I37" s="45" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="J37" s="21" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="K37" s="22" t="s">
         <v>50</v>
@@ -4609,13 +4612,13 @@
         <v>0.49763888888888891</v>
       </c>
       <c r="H38" s="21" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="I38" s="21" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="J38" s="48" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="K38" s="22" t="s">
         <v>50</v>
@@ -4652,13 +4655,13 @@
         <v>0.49934027777777779</v>
       </c>
       <c r="H39" s="21" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="J39" s="48" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="K39" s="22" t="s">
         <v>50</v>
@@ -4695,13 +4698,13 @@
         <v>0.50121527777777775</v>
       </c>
       <c r="H40" s="21" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="J40" s="48" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="K40" s="22" t="s">
         <v>50</v>
@@ -4738,13 +4741,13 @@
         <v>0.50292824074074072</v>
       </c>
       <c r="H41" s="46" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="I41" s="50" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="J41" s="49" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="K41" s="22" t="s">
         <v>50</v>
@@ -4781,13 +4784,13 @@
         <v>0.50474537037037037</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="I42" s="21" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="J42" s="22" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="K42" s="22" t="s">
         <v>50</v>
@@ -4824,13 +4827,13 @@
         <v>0.50670138888888883</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="I43" s="21" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="J43" s="48" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="K43" s="22" t="s">
         <v>50</v>
@@ -4867,13 +4870,13 @@
         <v>0.50885416666666672</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="I44" s="21" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="J44" s="48" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="K44" s="48" t="s">
         <v>50</v>
@@ -4910,13 +4913,13 @@
         <v>0.51206018518518526</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="I45" s="49" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="J45" s="48" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="K45" s="22" t="s">
         <v>50</v>
@@ -4953,13 +4956,13 @@
         <v>0.5136574074074074</v>
       </c>
       <c r="H46" s="49" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="I46" s="21" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="J46" s="48" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="K46" s="22" t="s">
         <v>50</v>
@@ -4996,13 +4999,13 @@
         <v>0.51543981481481482</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="J47" s="48" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="K47" s="22" t="s">
         <v>50</v>
@@ -5039,13 +5042,13 @@
         <v>0.51703703703703707</v>
       </c>
       <c r="H48" s="49" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="J48" s="48" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="K48" s="22" t="s">
         <v>50</v>
@@ -5082,13 +5085,13 @@
         <v>0.51885416666666673</v>
       </c>
       <c r="H49" s="21" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="I49" s="21" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="J49" s="48" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="K49" s="22" t="s">
         <v>50</v>
@@ -5125,13 +5128,13 @@
         <v>0.52046296296296302</v>
       </c>
       <c r="H50" s="21" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="J50" s="48" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="K50" s="22" t="s">
         <v>50</v>
@@ -5168,13 +5171,13 @@
         <v>0.52236111111111116</v>
       </c>
       <c r="H51" s="21" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="I51" s="21" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="J51" s="48" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="K51" s="22" t="s">
         <v>50</v>
@@ -5211,13 +5214,13 @@
         <v>0.52488425925925919</v>
       </c>
       <c r="H52" s="21" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="J52" s="48" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="K52" s="22" t="s">
         <v>50</v>
@@ -5254,13 +5257,13 @@
         <v>0.52700231481481474</v>
       </c>
       <c r="H53" s="21" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="I53" s="21" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="J53" s="48" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="K53" s="48" t="s">
         <v>50</v>
@@ -5297,13 +5300,13 @@
         <v>0.52986111111111112</v>
       </c>
       <c r="H54" s="21" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="I54" s="21" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="J54" s="48" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="K54" s="48" t="s">
         <v>50</v>
@@ -5340,13 +5343,13 @@
         <v>0.5320138888888889</v>
       </c>
       <c r="H55" s="21" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="I55" s="21" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="J55" s="48" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="K55" s="22" t="s">
         <v>50</v>
@@ -5383,13 +5386,13 @@
         <v>0.53622685185185182</v>
       </c>
       <c r="H56" s="21" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="I56" s="21" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="J56" s="48" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="K56" s="22" t="s">
         <v>50</v>
@@ -5426,13 +5429,13 @@
         <v>0.5387615740740741</v>
       </c>
       <c r="H57" s="21" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="I57" s="21" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="J57" s="48" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="K57" s="22" t="s">
         <v>50</v>
@@ -5469,13 +5472,13 @@
         <v>0.5408680555555555</v>
       </c>
       <c r="H58" s="21" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="I58" s="21" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="J58" s="48" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="K58" s="22" t="s">
         <v>50</v>
@@ -5512,13 +5515,13 @@
         <v>0.54289351851851853</v>
       </c>
       <c r="H59" s="21" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="I59" s="21" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="J59" s="48" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="K59" s="22" t="s">
         <v>50</v>
@@ -5555,13 +5558,13 @@
         <v>0.5449074074074074</v>
       </c>
       <c r="H60" s="21" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="I60" s="21" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="J60" s="48" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="K60" s="48" t="s">
         <v>50</v>

</xml_diff>